<commit_message>
Added log facility to gather information about errors + new coversion functions from xlsx
</commit_message>
<xml_diff>
--- a/inst/xls_xls_dic.xlsx
+++ b/inst/xls_xls_dic.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8414" uniqueCount="2411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8420" uniqueCount="2415">
   <si>
     <t>colname</t>
   </si>
@@ -7247,7 +7247,19 @@
     <t>q_59a:q_59d</t>
   </si>
   <si>
-    <t>µkat/l</t>
+    <t>U/L-&gt;U/l;ukat/l-&gt;µkat/l</t>
+  </si>
+  <si>
+    <t>g/L-&gt;g/l;g/dL-&gt;g/dl</t>
+  </si>
+  <si>
+    <t>mg/dL-&gt;mg/dl;umol/l-&gt;µmol/l</t>
+  </si>
+  <si>
+    <t>mg/dL-&gt;mg/dl</t>
+  </si>
+  <si>
+    <t>mg/dL-&gt;mg/dl;mg/Dl-&gt;mg/dl</t>
   </si>
 </sst>
 </file>
@@ -7754,8 +7766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="L123" sqref="L123"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="L202" sqref="L202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14888,7 +14900,6 @@
       <c r="K124" s="1" t="s">
         <v>2373</v>
       </c>
-      <c r="L124" s="1"/>
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
@@ -14946,7 +14957,7 @@
       <c r="K125" s="1" t="s">
         <v>2373</v>
       </c>
-      <c r="L125" s="1"/>
+      <c r="L125" s="44"/>
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
@@ -15061,7 +15072,9 @@
       <c r="K127" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L127" s="1"/>
+      <c r="L127" s="44" t="s">
+        <v>2411</v>
+      </c>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
@@ -15292,7 +15305,9 @@
       <c r="K131" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L131" s="1"/>
+      <c r="L131" s="44" t="s">
+        <v>2412</v>
+      </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
       <c r="O131" s="1"/>
@@ -15523,7 +15538,9 @@
       <c r="K135" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L135" s="1"/>
+      <c r="L135" s="44" t="s">
+        <v>2413</v>
+      </c>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
       <c r="O135" s="1"/>
@@ -15754,7 +15771,9 @@
       <c r="K139" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L139" s="1"/>
+      <c r="L139" s="44" t="s">
+        <v>2413</v>
+      </c>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
       <c r="O139" s="1"/>
@@ -15985,7 +16004,9 @@
       <c r="K143" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L143" s="1"/>
+      <c r="L143" s="44" t="s">
+        <v>2413</v>
+      </c>
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
       <c r="O143" s="1"/>
@@ -16216,7 +16237,9 @@
       <c r="K147" s="1" t="s">
         <v>2403</v>
       </c>
-      <c r="L147" s="1"/>
+      <c r="L147" s="44" t="s">
+        <v>2414</v>
+      </c>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
       <c r="O147" s="1"/>

</xml_diff>

<commit_message>
Incremental work on converting specialists
</commit_message>
<xml_diff>
--- a/inst/xls_xls_dic.xlsx
+++ b/inst/xls_xls_dic.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8646" uniqueCount="2420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8647" uniqueCount="2422">
   <si>
     <t>colname</t>
   </si>
@@ -7275,6 +7275,12 @@
   </si>
   <si>
     <t>GP-&gt;General Practitioner;general practicioner-&gt;General Practitioner;general pracitioner-&gt;General Practitioner;general and familiar medicine (gp)-&gt;General Practitioner;general practitioner n-&gt;General Practitioner;general practioner-&gt;General Practitioner;general practicer-&gt;General Practitioner;practitioner-&gt;General Practitioner;family doctor-&gt;General Practitioner;ftr-&gt;!;internal medicen-&gt;internal medicine;internal medixcine-&gt;internal medicine;interna medicine-&gt;internal medicine;neurosurgery-&gt;neurosurgeon;ortopedist-&gt;Orthopaedist;pneumolog-&gt;Pneumologist;neurosurgen-&gt;Neurosurgeon;neurosurgeon no-&gt;Neurosurgeon;lor-&gt;!;physiotherayist-&gt;!other;orthopedic surgeon-&gt;!Orthopaedist;orthopedist hospital-&gt;Orthopaedist;orthopediest-&gt;Orthopaedist;orthopedist n-&gt;Orthopaedist;neurology-&gt;Neurologist;second neurologist-&gt;Neurologist;phoniatrist/ent-&gt;!;ent-&gt;Ear-Nose-Throat Doctor (ENT);ear nose troat doctor-&gt;Ear-Nose-Throat Doctor (ENT);ent n-&gt;Ear-Nose-Throat Doctor (ENT);ear-nose-throat-doctor-&gt;Ear-Nose-Throat Doctor (ENT);ortopaedist-&gt;Orthopaedist;nf-&gt;NA;ent y-&gt;Ear-Nose-Throat Doctor (ENT);ear-nose-troat-doctor-&gt;Ear-Nose-Throat Doctor (ENT);neurologist (clinic) y-&gt;Neurologist;neurologist clinic-&gt;Neurologist;neurologist (hospital)-&gt;Neurologist;neurologist n-&gt;Neurologist;first neurologist-&gt;Neurologist;neurologist, n-&gt;Neurologist;neurologisy y-&gt;Neurologist;neruologist-&gt;Neurologist;neurlogist-&gt;Neurologist;neurologist no-&gt;Neurologist;orthopaedist n-&gt;Orthopaedist;neurologist (clinic)-&gt;Neurologist;neurologist c y-&gt;Neurologist;second neurology-&gt;Neurologist;neurologist in clinic-&gt;Neurologist;neurologist c  y-&gt;Neurologist;neurology,yes-&gt;Neurologist;neurologist 8th specialist-&gt;Neurologist;neurologist c-&gt;Neurologist;neurologist c n-&gt;Neurologist;orthopedist-&gt;Orthopaedist;orthopedic-&gt;Orthopaedist;ortophedist-&gt;Orthopaedist;neurologist y-&gt;Neurologist;dentist-&gt;!other;dentist n-&gt;!other;surgeon-&gt;General surgeon;vascular surgeon-&gt;!General surgeon;rehabilitation-&gt;Rehabilitation specialist;physical medicine and rehabilitation-&gt;Rehabilitation specialist;rheumathologist-&gt;Rheumatologist;reumathologist-&gt;Rheumatologist;reumatologist-&gt;Rheumatologist;hematologist-&gt;!other;surgeon /ent-&gt;!general surgeon;otorhinolaryngology (ent)-&gt;!other;psychologist-&gt;!other;pm&amp;r-&gt;!Psychiatrist;41913-&gt;!;internist-&gt;!other;laryngologist-&gt;!other;kardiologist-&gt;Cardiologist;phoniater,no-&gt;!other;no-&gt;NA;pulmonologist-&gt;!Pneumologist;otolaryngologist-&gt;!other;no other-&gt;NA;clinic-&gt;!;orthodontist n-&gt;!other;physiatrist-&gt;Psychiatrist;gastroenterologist-&gt;!other;first-&gt;!;second-&gt;!;mhh-&gt;!;hospital-&gt;!;no diagnosis till consultation-&gt;NA;university hostpital desden-&gt;!;pm&amp;r (physiatrist)-&gt;Psychiatrist</t>
+  </si>
+  <si>
+    <t>yes-&gt;!</t>
+  </si>
+  <si>
+    <t>one_specialist</t>
   </si>
 </sst>
 </file>
@@ -7775,8 +7781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A516" workbookViewId="0">
-      <selection activeCell="J536" sqref="J536"/>
+    <sheetView tabSelected="1" topLeftCell="A498" workbookViewId="0">
+      <selection activeCell="L514" sqref="L514"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -34163,7 +34169,9 @@
       <c r="K461" s="1" t="s">
         <v>2351</v>
       </c>
-      <c r="L461" s="1"/>
+      <c r="L461" s="1" t="s">
+        <v>2420</v>
+      </c>
       <c r="M461" s="1"/>
       <c r="N461" s="1"/>
       <c r="O461" s="1"/>
@@ -34220,7 +34228,9 @@
       <c r="K462" s="1" t="s">
         <v>2351</v>
       </c>
-      <c r="L462" s="1"/>
+      <c r="L462" s="1" t="s">
+        <v>2420</v>
+      </c>
       <c r="M462" s="1"/>
       <c r="N462" s="1"/>
       <c r="O462" s="1"/>
@@ -37208,7 +37218,7 @@
         <v>1063</v>
       </c>
       <c r="K514" s="1" t="s">
-        <v>2343</v>
+        <v>2421</v>
       </c>
       <c r="L514" s="1" t="s">
         <v>2419</v>
@@ -37743,7 +37753,7 @@
         <v>1072</v>
       </c>
       <c r="K524" s="1" t="s">
-        <v>2343</v>
+        <v>2421</v>
       </c>
       <c r="L524" s="1" t="str">
         <f>L514</f>
@@ -38327,7 +38337,7 @@
         <v>1087</v>
       </c>
       <c r="K535" s="1" t="s">
-        <v>2343</v>
+        <v>2421</v>
       </c>
       <c r="L535" s="1" t="str">
         <f>L524</f>
@@ -38360,42 +38370,40 @@
       <c r="C536" t="s">
         <v>545</v>
       </c>
-      <c r="D536" s="3" t="e">
+      <c r="D536" s="3" t="str">
         <f t="shared" ca="1" si="548"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="E536" t="s">
         <v>8</v>
       </c>
-      <c r="F536" s="3" t="e">
+      <c r="F536" s="3" t="str">
         <f t="shared" ca="1" si="544"/>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="G536" t="s">
         <v>1886</v>
       </c>
-      <c r="H536" s="3" t="e">
+      <c r="H536" s="3" t="str">
         <f t="shared" ca="1" si="545"/>
-        <v>#N/A</v>
-      </c>
-      <c r="J536" s="1" t="s">
-        <v>1897</v>
-      </c>
-      <c r="Q536" s="1" t="e">
+        <v/>
+      </c>
+      <c r="J536" s="1"/>
+      <c r="Q536" s="1" t="str">
         <f t="shared" ca="1" si="546"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R536" t="e">
+        <v/>
+      </c>
+      <c r="R536" t="str">
         <f t="shared" ref="R536:T536" ca="1" si="560">IF(Q536&lt;&gt;"",INDEX(INDIRECT(R$2),$Q536),"")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S536" t="e">
+        <v/>
+      </c>
+      <c r="S536" t="str">
         <f t="shared" ca="1" si="560"/>
-        <v>#N/A</v>
-      </c>
-      <c r="T536" t="e">
+        <v/>
+      </c>
+      <c r="T536" t="str">
         <f t="shared" ca="1" si="560"/>
-        <v>#N/A</v>
+        <v/>
       </c>
     </row>
     <row r="537" spans="1:20">

</xml_diff>

<commit_message>
first version of merging all the databases
</commit_message>
<xml_diff>
--- a/inst/xls_xls_dic.xlsx
+++ b/inst/xls_xls_dic.xlsx
@@ -7784,8 +7784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A535" workbookViewId="0">
-      <selection activeCell="L574" sqref="L574"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="I230" sqref="I230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Many small fixes to the conversion between formats
</commit_message>
<xml_diff>
--- a/inst/xls_xls_dic.xlsx
+++ b/inst/xls_xls_dic.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8648" uniqueCount="2423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8651" uniqueCount="2423">
   <si>
     <t>colname</t>
   </si>
@@ -7187,9 +7187,6 @@
     <t>1-&gt;4;2-&gt;2;3-&gt;1;4-&gt;3</t>
   </si>
   <si>
-    <t>3-&gt;NF</t>
-  </si>
-  <si>
     <t>1-&gt;2;2-&gt;1;3-&gt;NF</t>
   </si>
   <si>
@@ -7283,7 +7280,10 @@
     <t>one_specialist</t>
   </si>
   <si>
-    <t>ANTC-&gt;ANTA;J-&gt;JENA</t>
+    <t>ANTC-&gt;ANTA;J-&gt;JENA;Hann-&gt;HANN;Con-&gt;HANN</t>
+  </si>
+  <si>
+    <t>1-&gt;!2;2-&gt;1</t>
   </si>
 </sst>
 </file>
@@ -7784,8 +7784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T574"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="I230" sqref="I230"/>
+    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
+      <selection activeCell="D555" sqref="D555"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -12333,7 +12333,7 @@
         <v>548</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>2390</v>
+        <v>790</v>
       </c>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
@@ -12392,7 +12392,7 @@
         <v>548</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
@@ -13865,7 +13865,7 @@
         <v>725</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="L106" s="1"/>
       <c r="M106" s="1"/>
@@ -13979,7 +13979,7 @@
         <v>727</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="L108" s="1"/>
       <c r="M108" s="1"/>
@@ -14853,13 +14853,13 @@
       </c>
       <c r="I123" s="1"/>
       <c r="J123" s="1" t="s">
+        <v>2400</v>
+      </c>
+      <c r="K123" s="1" t="s">
         <v>2401</v>
       </c>
-      <c r="K123" s="1" t="s">
-        <v>2402</v>
-      </c>
       <c r="L123" s="38" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
@@ -15085,13 +15085,13 @@
       </c>
       <c r="I127" s="1"/>
       <c r="J127" s="1" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L127" s="38" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
@@ -15318,13 +15318,13 @@
       </c>
       <c r="I131" s="1"/>
       <c r="J131" s="1" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L131" s="38" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
@@ -15551,13 +15551,13 @@
       </c>
       <c r="I135" s="1"/>
       <c r="J135" s="1" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L135" s="38" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
@@ -15784,13 +15784,13 @@
       </c>
       <c r="I139" s="1"/>
       <c r="J139" s="1" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L139" s="38" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
@@ -16017,13 +16017,13 @@
       </c>
       <c r="I143" s="1"/>
       <c r="J143" s="1" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L143" s="38" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
@@ -16250,13 +16250,13 @@
       </c>
       <c r="I147" s="1"/>
       <c r="J147" s="1" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="L147" s="38" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
@@ -17338,7 +17338,7 @@
         <v>548</v>
       </c>
       <c r="L166" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
@@ -17397,7 +17397,7 @@
         <v>548</v>
       </c>
       <c r="L167" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
@@ -17456,7 +17456,7 @@
         <v>548</v>
       </c>
       <c r="L168" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
@@ -17515,7 +17515,7 @@
         <v>548</v>
       </c>
       <c r="L169" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
@@ -17574,7 +17574,7 @@
         <v>548</v>
       </c>
       <c r="L170" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M170" s="1"/>
       <c r="N170" s="1"/>
@@ -17633,7 +17633,7 @@
         <v>548</v>
       </c>
       <c r="L171" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M171" s="1"/>
       <c r="N171" s="1"/>
@@ -17692,7 +17692,7 @@
         <v>548</v>
       </c>
       <c r="L172" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M172" s="1"/>
       <c r="N172" s="1"/>
@@ -17751,7 +17751,7 @@
         <v>548</v>
       </c>
       <c r="L173" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M173" s="1"/>
       <c r="N173" s="1"/>
@@ -17867,7 +17867,7 @@
         <v>548</v>
       </c>
       <c r="L175" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M175" s="1"/>
       <c r="N175" s="1"/>
@@ -17926,7 +17926,7 @@
         <v>548</v>
       </c>
       <c r="L176" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M176" s="1"/>
       <c r="N176" s="1"/>
@@ -17985,7 +17985,7 @@
         <v>548</v>
       </c>
       <c r="L177" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M177" s="1"/>
       <c r="N177" s="1"/>
@@ -18044,7 +18044,7 @@
         <v>2339</v>
       </c>
       <c r="L178" s="1" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="M178" s="1"/>
       <c r="N178" s="11"/>
@@ -18211,7 +18211,7 @@
         <v>2339</v>
       </c>
       <c r="L181" s="1" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="M181" s="1"/>
       <c r="N181" s="12"/>
@@ -18594,7 +18594,7 @@
         <v>548</v>
       </c>
       <c r="L188" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M188" s="1"/>
       <c r="N188" s="1"/>
@@ -18708,7 +18708,7 @@
         <v>548</v>
       </c>
       <c r="L190" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M190" s="1"/>
       <c r="N190" s="1"/>
@@ -18719,7 +18719,7 @@
         <v>276</v>
       </c>
       <c r="R190" t="str">
-        <f t="shared" ref="R190:T190" ca="1" si="190">IF(Q190&lt;&gt;"",INDEX(INDIRECT(R$2),$Q190),"")</f>
+        <f t="shared" ref="R190:T191" ca="1" si="190">IF(Q190&lt;&gt;"",INDEX(INDIRECT(R$2),$Q190),"")</f>
         <v>Cancer treatment – Radiotherapy</v>
       </c>
       <c r="S190" t="str">
@@ -18763,8 +18763,12 @@
       <c r="J191" s="1" t="s">
         <v>884</v>
       </c>
-      <c r="K191" s="1"/>
-      <c r="L191" s="1"/>
+      <c r="K191" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="L191" s="1" t="s">
+        <v>2422</v>
+      </c>
       <c r="M191" s="1"/>
       <c r="N191" s="1"/>
       <c r="O191" s="1"/>
@@ -18778,7 +18782,7 @@
         <v>Cancer treatment – Radiotherapy of head or neck</v>
       </c>
       <c r="S191" t="str">
-        <f t="shared" ca="1" si="191"/>
+        <f t="shared" ca="1" si="190"/>
         <v>integer</v>
       </c>
       <c r="T191" t="str">
@@ -18822,7 +18826,7 @@
         <v>548</v>
       </c>
       <c r="L192" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M192" s="1"/>
       <c r="N192" s="1"/>
@@ -18878,10 +18882,10 @@
         <v>886</v>
       </c>
       <c r="K193" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="L193" s="1" t="s">
         <v>2397</v>
-      </c>
-      <c r="L193" s="1" t="s">
-        <v>2398</v>
       </c>
       <c r="M193" s="1"/>
       <c r="N193" s="1"/>
@@ -18940,7 +18944,7 @@
         <v>548</v>
       </c>
       <c r="L194" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M194" s="1"/>
       <c r="N194" s="1"/>
@@ -18996,10 +19000,10 @@
         <v>888</v>
       </c>
       <c r="K195" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="L195" s="1" t="s">
         <v>2397</v>
-      </c>
-      <c r="L195" s="1" t="s">
-        <v>2398</v>
       </c>
       <c r="M195" s="1"/>
       <c r="N195" s="1"/>
@@ -19055,10 +19059,10 @@
         <v>889</v>
       </c>
       <c r="K196" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="L196" s="1" t="s">
         <v>2397</v>
-      </c>
-      <c r="L196" s="1" t="s">
-        <v>2398</v>
       </c>
       <c r="M196" s="1"/>
       <c r="N196" s="1"/>
@@ -19117,7 +19121,7 @@
         <v>548</v>
       </c>
       <c r="L197" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M197" s="1"/>
       <c r="N197" s="1"/>
@@ -19231,7 +19235,7 @@
         <v>548</v>
       </c>
       <c r="L199" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M199" s="1"/>
       <c r="N199" s="1"/>
@@ -19345,7 +19349,7 @@
         <v>548</v>
       </c>
       <c r="L201" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M201" s="1"/>
       <c r="N201" s="1"/>
@@ -19516,7 +19520,7 @@
         <v>548</v>
       </c>
       <c r="L204" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M204" s="1"/>
       <c r="N204" s="1"/>
@@ -19630,7 +19634,7 @@
         <v>548</v>
       </c>
       <c r="L206" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M206" s="1"/>
       <c r="N206" s="1"/>
@@ -19744,7 +19748,7 @@
         <v>548</v>
       </c>
       <c r="L208" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M208" s="1"/>
       <c r="N208" s="1"/>
@@ -19858,7 +19862,7 @@
         <v>548</v>
       </c>
       <c r="L210" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M210" s="1"/>
       <c r="N210" s="1"/>
@@ -19972,7 +19976,7 @@
         <v>548</v>
       </c>
       <c r="L212" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M212" s="1"/>
       <c r="N212" s="1"/>
@@ -20086,7 +20090,7 @@
         <v>548</v>
       </c>
       <c r="L214" s="1" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="M214" s="1"/>
       <c r="N214" s="1"/>
@@ -20310,7 +20314,7 @@
         <v>2343</v>
       </c>
       <c r="L218" s="1" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="M218" s="1"/>
       <c r="N218" s="1"/>
@@ -20424,7 +20428,7 @@
         <v>2343</v>
       </c>
       <c r="L220" s="1" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="M220" s="1"/>
       <c r="N220" s="1"/>
@@ -20538,7 +20542,7 @@
         <v>2343</v>
       </c>
       <c r="L222" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="M222" s="1"/>
       <c r="N222" s="1"/>
@@ -20652,7 +20656,7 @@
         <v>2343</v>
       </c>
       <c r="L224" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="M224" s="1"/>
       <c r="N224" s="1"/>
@@ -20766,7 +20770,7 @@
         <v>2343</v>
       </c>
       <c r="L226" s="1" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="M226" s="1"/>
       <c r="N226" s="1"/>
@@ -20880,7 +20884,7 @@
         <v>548</v>
       </c>
       <c r="L228" s="1" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="M228" s="1"/>
       <c r="N228" s="1"/>
@@ -22753,7 +22757,7 @@
       </c>
       <c r="I261" s="1"/>
       <c r="J261" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K261" s="1" t="s">
         <v>2346</v>
@@ -22810,7 +22814,7 @@
       </c>
       <c r="I262" s="1"/>
       <c r="J262" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K262" s="1" t="s">
         <v>2373</v>
@@ -22867,7 +22871,7 @@
       </c>
       <c r="I263" s="1"/>
       <c r="J263" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K263" s="1" t="s">
         <v>2373</v>
@@ -22924,7 +22928,7 @@
       </c>
       <c r="I264" s="1"/>
       <c r="J264" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K264" s="1" t="s">
         <v>2373</v>
@@ -22981,7 +22985,7 @@
       </c>
       <c r="I265" s="1"/>
       <c r="J265" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K265" s="1" t="s">
         <v>2373</v>
@@ -23038,7 +23042,7 @@
       </c>
       <c r="I266" s="1"/>
       <c r="J266" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K266" s="1" t="s">
         <v>2373</v>
@@ -23095,7 +23099,7 @@
       </c>
       <c r="I267" s="1"/>
       <c r="J267" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K267" s="1" t="s">
         <v>2373</v>
@@ -23152,7 +23156,7 @@
       </c>
       <c r="I268" s="1"/>
       <c r="J268" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K268" s="1" t="s">
         <v>2373</v>
@@ -23209,7 +23213,7 @@
       </c>
       <c r="I269" s="1"/>
       <c r="J269" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K269" s="1" t="s">
         <v>2373</v>
@@ -23266,7 +23270,7 @@
       </c>
       <c r="I270" s="1"/>
       <c r="J270" s="37" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="K270" s="1" t="s">
         <v>2373</v>
@@ -24577,7 +24581,7 @@
       </c>
       <c r="I293" s="1"/>
       <c r="J293" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K293" s="1" t="s">
         <v>2348</v>
@@ -24634,7 +24638,7 @@
       </c>
       <c r="I294" s="1"/>
       <c r="J294" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K294" s="1" t="s">
         <v>2373</v>
@@ -24691,7 +24695,7 @@
       </c>
       <c r="I295" s="1"/>
       <c r="J295" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K295" s="1" t="s">
         <v>2373</v>
@@ -24748,7 +24752,7 @@
       </c>
       <c r="I296" s="1"/>
       <c r="J296" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K296" s="1" t="s">
         <v>2373</v>
@@ -24805,7 +24809,7 @@
       </c>
       <c r="I297" s="1"/>
       <c r="J297" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K297" s="1" t="s">
         <v>2373</v>
@@ -24862,7 +24866,7 @@
       </c>
       <c r="I298" s="1"/>
       <c r="J298" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K298" s="1" t="s">
         <v>2373</v>
@@ -24919,7 +24923,7 @@
       </c>
       <c r="I299" s="1"/>
       <c r="J299" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K299" s="1" t="s">
         <v>2373</v>
@@ -24976,7 +24980,7 @@
       </c>
       <c r="I300" s="1"/>
       <c r="J300" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K300" s="1" t="s">
         <v>2373</v>
@@ -25033,7 +25037,7 @@
       </c>
       <c r="I301" s="1"/>
       <c r="J301" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K301" s="1" t="s">
         <v>2373</v>
@@ -25090,7 +25094,7 @@
       </c>
       <c r="I302" s="1"/>
       <c r="J302" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K302" s="1" t="s">
         <v>2373</v>
@@ -25147,7 +25151,7 @@
       </c>
       <c r="I303" s="1"/>
       <c r="J303" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K303" s="1" t="s">
         <v>2373</v>
@@ -25204,7 +25208,7 @@
       </c>
       <c r="I304" s="1"/>
       <c r="J304" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K304" s="1" t="s">
         <v>2373</v>
@@ -25261,7 +25265,7 @@
       </c>
       <c r="I305" s="1"/>
       <c r="J305" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K305" s="1" t="s">
         <v>2373</v>
@@ -25318,7 +25322,7 @@
       </c>
       <c r="I306" s="1"/>
       <c r="J306" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K306" s="1" t="s">
         <v>2373</v>
@@ -25375,7 +25379,7 @@
       </c>
       <c r="I307" s="1"/>
       <c r="J307" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K307" s="1" t="s">
         <v>2373</v>
@@ -25432,7 +25436,7 @@
       </c>
       <c r="I308" s="1"/>
       <c r="J308" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K308" s="1" t="s">
         <v>2373</v>
@@ -25489,7 +25493,7 @@
       </c>
       <c r="I309" s="1"/>
       <c r="J309" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K309" s="1" t="s">
         <v>2373</v>
@@ -25546,7 +25550,7 @@
       </c>
       <c r="I310" s="1"/>
       <c r="J310" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K310" s="1" t="s">
         <v>2373</v>
@@ -25603,7 +25607,7 @@
       </c>
       <c r="I311" s="1"/>
       <c r="J311" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K311" s="1" t="s">
         <v>2373</v>
@@ -25660,7 +25664,7 @@
       </c>
       <c r="I312" s="1"/>
       <c r="J312" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K312" s="1" t="s">
         <v>2373</v>
@@ -25717,7 +25721,7 @@
       </c>
       <c r="I313" s="1"/>
       <c r="J313" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K313" s="1" t="s">
         <v>2373</v>
@@ -25774,7 +25778,7 @@
       </c>
       <c r="I314" s="1"/>
       <c r="J314" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K314" s="1" t="s">
         <v>2373</v>
@@ -25831,7 +25835,7 @@
       </c>
       <c r="I315" s="1"/>
       <c r="J315" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K315" s="1" t="s">
         <v>2373</v>
@@ -25888,7 +25892,7 @@
       </c>
       <c r="I316" s="1"/>
       <c r="J316" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K316" s="1" t="s">
         <v>2373</v>
@@ -25945,7 +25949,7 @@
       </c>
       <c r="I317" s="1"/>
       <c r="J317" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K317" s="1" t="s">
         <v>2373</v>
@@ -26002,7 +26006,7 @@
       </c>
       <c r="I318" s="1"/>
       <c r="J318" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K318" s="1" t="s">
         <v>2373</v>
@@ -26059,7 +26063,7 @@
       </c>
       <c r="I319" s="1"/>
       <c r="J319" s="1" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="K319" s="1" t="s">
         <v>2373</v>
@@ -26296,7 +26300,7 @@
         <v>929</v>
       </c>
       <c r="K323" s="1" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="L323" s="1"/>
       <c r="M323" s="1"/>
@@ -34173,7 +34177,7 @@
         <v>2351</v>
       </c>
       <c r="L461" s="1" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="M461" s="1"/>
       <c r="N461" s="1"/>
@@ -34232,7 +34236,7 @@
         <v>2351</v>
       </c>
       <c r="L462" s="1" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="M462" s="1"/>
       <c r="N462" s="1"/>
@@ -37221,10 +37225,10 @@
         <v>1063</v>
       </c>
       <c r="K514" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="L514" s="1" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="Q514" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37327,7 +37331,7 @@
         <v>548</v>
       </c>
       <c r="L516" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q516" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37381,7 +37385,7 @@
         <v>548</v>
       </c>
       <c r="L517" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q517" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37435,7 +37439,7 @@
         <v>548</v>
       </c>
       <c r="L518" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q518" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37489,7 +37493,7 @@
         <v>548</v>
       </c>
       <c r="L519" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q519" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37543,7 +37547,7 @@
         <v>548</v>
       </c>
       <c r="L520" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q520" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37597,7 +37601,7 @@
         <v>548</v>
       </c>
       <c r="L521" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q521" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37651,7 +37655,7 @@
         <v>548</v>
       </c>
       <c r="L522" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q522" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37705,7 +37709,7 @@
         <v>548</v>
       </c>
       <c r="L523" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q523" s="1">
         <f t="shared" ca="1" si="478"/>
@@ -37756,7 +37760,7 @@
         <v>1072</v>
       </c>
       <c r="K524" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="L524" s="1" t="str">
         <f>L514</f>
@@ -37811,7 +37815,7 @@
         <v>1073</v>
       </c>
       <c r="K525" s="1" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="Q525" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -37911,7 +37915,7 @@
         <v>548</v>
       </c>
       <c r="L527" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q527" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -37965,7 +37969,7 @@
         <v>548</v>
       </c>
       <c r="L528" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q528" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38019,7 +38023,7 @@
         <v>548</v>
       </c>
       <c r="L529" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q529" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38073,7 +38077,7 @@
         <v>548</v>
       </c>
       <c r="L530" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q530" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38127,7 +38131,7 @@
         <v>548</v>
       </c>
       <c r="L531" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q531" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38181,7 +38185,7 @@
         <v>548</v>
       </c>
       <c r="L532" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q532" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38235,7 +38239,7 @@
         <v>548</v>
       </c>
       <c r="L533" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q533" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38289,7 +38293,7 @@
         <v>548</v>
       </c>
       <c r="L534" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q534" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38340,7 +38344,7 @@
         <v>1087</v>
       </c>
       <c r="K535" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="L535" s="1" t="str">
         <f>L524</f>
@@ -38845,6 +38849,9 @@
       <c r="J545" s="1" t="s">
         <v>1922</v>
       </c>
+      <c r="K545" s="1" t="s">
+        <v>2342</v>
+      </c>
       <c r="Q545" s="1">
         <f t="shared" ca="1" si="546"/>
         <v>554</v>
@@ -38897,7 +38904,7 @@
         <v>548</v>
       </c>
       <c r="L546" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q546" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -38951,7 +38958,7 @@
         <v>548</v>
       </c>
       <c r="L547" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q547" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39005,7 +39012,7 @@
         <v>548</v>
       </c>
       <c r="L548" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q548" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39059,7 +39066,7 @@
         <v>548</v>
       </c>
       <c r="L549" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q549" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39113,7 +39120,7 @@
         <v>548</v>
       </c>
       <c r="L550" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q550" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39167,7 +39174,7 @@
         <v>548</v>
       </c>
       <c r="L551" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q551" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39221,7 +39228,7 @@
         <v>548</v>
       </c>
       <c r="L552" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q552" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -39275,7 +39282,7 @@
         <v>548</v>
       </c>
       <c r="L553" s="1" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="Q553" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -40285,7 +40292,7 @@
         <v>546</v>
       </c>
       <c r="K573" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="Q573" s="1">
         <f t="shared" ca="1" si="546"/>
@@ -40339,7 +40346,7 @@
         <v>2351</v>
       </c>
       <c r="L574" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="Q574" s="1" t="e">
         <f t="shared" ca="1" si="546"/>

</xml_diff>